<commit_message>
UPDATE MVC JURUSAN AKL
</commit_message>
<xml_diff>
--- a/temp_doc/Soal.xlsx
+++ b/temp_doc/Soal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.5admin/temp_doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cbt2.5admin\temp_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51021A9C-1E66-164E-8145-5B7FBCDDA5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5367136-6DFC-4F7C-8A78-C33DE262D7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{6ACE4BE8-8983-534E-97D6-0435C912BA51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6ACE4BE8-8983-534E-97D6-0435C912BA51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,15 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
-    <t>1. Dalam menyusun suatu program,langkah pertama yang harus di lakkukan adalah :</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>3. Pseudocode yang di gunakan pada penulisan algoritma berupa :</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -267,6 +261,12 @@
   </si>
   <si>
     <t>Semua benar</t>
+  </si>
+  <si>
+    <t>Dalam menyusun suatu program,langkah pertama yang harus di lakkukan adalah :</t>
+  </si>
+  <si>
+    <t>Pseudocode yang di gunakan pada penulisan algoritma berupa :</t>
   </si>
 </sst>
 </file>
@@ -644,272 +644,272 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.125" customWidth="1"/>
     <col min="2" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="3" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="2" t="s">
+    <row r="10" spans="1:7" ht="57" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -918,7 +918,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -927,7 +927,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -936,7 +936,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -945,7 +945,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -954,7 +954,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -963,7 +963,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -972,7 +972,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -981,7 +981,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -990,7 +990,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -999,7 +999,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1008,7 +1008,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1017,7 +1017,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1026,7 +1026,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1035,7 +1035,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1044,7 +1044,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1053,7 +1053,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1062,7 +1062,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1071,7 +1071,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1080,7 +1080,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1089,7 +1089,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1098,7 +1098,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1107,7 +1107,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1116,7 +1116,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1125,7 +1125,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1134,7 +1134,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1143,7 +1143,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1152,7 +1152,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1161,7 +1161,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1170,7 +1170,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1179,7 +1179,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1188,7 +1188,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1197,7 +1197,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1206,7 +1206,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1215,7 +1215,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1224,7 +1224,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1233,7 +1233,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1242,7 +1242,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1251,7 +1251,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1260,7 +1260,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1269,7 +1269,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1278,7 +1278,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1287,7 +1287,7 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1296,7 +1296,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1305,7 +1305,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1314,7 +1314,7 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1323,7 +1323,7 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1332,7 +1332,7 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1341,7 +1341,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1350,7 +1350,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1359,7 +1359,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1368,7 +1368,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1377,7 +1377,7 @@
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1386,7 +1386,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1395,7 +1395,7 @@
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1404,7 +1404,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1413,7 +1413,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1422,7 +1422,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1431,7 +1431,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1440,7 +1440,7 @@
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1449,7 +1449,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1458,7 +1458,7 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1467,7 +1467,7 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1476,7 +1476,7 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1485,7 +1485,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1494,7 +1494,7 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1503,7 +1503,7 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1512,7 +1512,7 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -1521,7 +1521,7 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -1530,7 +1530,7 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -1539,7 +1539,7 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -1548,7 +1548,7 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -1557,7 +1557,7 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -1566,7 +1566,7 @@
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -1575,7 +1575,7 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -1584,7 +1584,7 @@
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -1593,7 +1593,7 @@
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -1602,7 +1602,7 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -1611,7 +1611,7 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -1620,7 +1620,7 @@
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -1629,7 +1629,7 @@
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -1638,7 +1638,7 @@
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -1647,7 +1647,7 @@
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -1656,7 +1656,7 @@
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -1665,7 +1665,7 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -1674,7 +1674,7 @@
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -1683,7 +1683,7 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -1692,7 +1692,7 @@
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -1701,7 +1701,7 @@
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -1710,7 +1710,7 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -1732,36 +1732,36 @@
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>